<commit_message>
change 2 on excel
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -1,11 +1,10 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21328"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D6BF6D83-5A2B-41CB-84A5-70D182444948}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
+  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+  <workbookPr filterPrivacy="1" defaultThemeVersion="164011"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-105" yWindow="-105" windowWidth="23250" windowHeight="12570"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
@@ -20,18 +19,21 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="2" uniqueCount="2">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="4" uniqueCount="3">
   <si>
     <t>Hello</t>
   </si>
   <si>
     <t>World</t>
   </si>
+  <si>
+    <t xml:space="preserve">Hi </t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" mc:Ignorable="x14ac x16r2">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -342,16 +344,16 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:B1"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B1" sqref="B1"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -359,6 +361,14 @@
         <v>1</v>
       </c>
     </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" t="s">
+        <v>1</v>
+      </c>
+    </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>